<commit_message>
Update screening data - 2025-06-11 08:15:10
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -798,11 +798,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>qwerty</t>
-        </is>
-      </c>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:38:34
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3801,7 +3801,11 @@
           <t>dqqws</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>dasda</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:40:35
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3796,16 +3796,8 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>dqqws</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>dasda</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:46:45
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3796,7 +3796,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>abc</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:47:20
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3801,7 +3801,11 @@
           <t>abc</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>qwe</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:48:12
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3796,16 +3796,8 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>abc</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>qwe</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:49:05
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3796,7 +3796,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 11:49:32
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3796,11 +3796,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>coco</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 12:27:52
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3823,73 +3823,77 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr">
+      <c r="D21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
         <is>
           <t>234</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
       <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr">
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr">
         <is>
           <t>insufficient sample size, poor methodology</t>
         </is>
       </c>
-      <c r="I21" t="inlineStr"/>
       <c r="J21" t="inlineStr"/>
-      <c r="K21" t="inlineStr">
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr">
         <is>
           <t>not relevant, poor methodology</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr"/>
       <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
-      <c r="R21" t="inlineStr">
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr">
         <is>
           <t>poor methodology, insufficient sample size</t>
         </is>
       </c>
-      <c r="S21" t="inlineStr"/>
-      <c r="T21" t="inlineStr">
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr">
         <is>
           <t>not relevant</t>
         </is>
       </c>
-      <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
-      <c r="W21" t="inlineStr">
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr">
         <is>
           <t>not relevant, poor methodology</t>
         </is>
       </c>
-      <c r="X21" t="inlineStr">
+      <c r="Y21" t="inlineStr">
         <is>
           <t>not relevant</t>
         </is>
       </c>
-      <c r="Y21" t="inlineStr"/>
       <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr">
+      <c r="AA21" t="inlineStr"/>
+      <c r="AB21" t="inlineStr">
         <is>
           <t>insufficient sample size, poor methodology</t>
         </is>
       </c>
-      <c r="AB21" t="inlineStr"/>
       <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr"/>
-      <c r="AG21" t="inlineStr">
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr">
         <is>
           <t>poor methodology</t>
         </is>
       </c>
-      <c r="AH21" t="inlineStr"/>
       <c r="AI21" t="inlineStr"/>
     </row>
     <row r="22">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 12:29:43
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3823,78 +3823,82 @@
         </is>
       </c>
       <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>coco</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr"/>
+      <c r="F21" t="inlineStr">
         <is>
           <t>234</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>23</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr"/>
-      <c r="I21" t="inlineStr">
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr">
         <is>
           <t>insufficient sample size, poor methodology</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr"/>
       <c r="K21" t="inlineStr"/>
-      <c r="L21" t="inlineStr">
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
         <is>
           <t>not relevant, poor methodology</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr"/>
       <c r="P21" t="inlineStr"/>
       <c r="Q21" t="inlineStr"/>
       <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr">
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr">
         <is>
           <t>poor methodology, insufficient sample size</t>
         </is>
       </c>
-      <c r="T21" t="inlineStr"/>
-      <c r="U21" t="inlineStr">
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr">
         <is>
           <t>not relevant</t>
         </is>
       </c>
-      <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
-      <c r="X21" t="inlineStr">
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr">
         <is>
           <t>not relevant, poor methodology</t>
         </is>
       </c>
-      <c r="Y21" t="inlineStr">
+      <c r="Z21" t="inlineStr">
         <is>
           <t>not relevant</t>
         </is>
       </c>
-      <c r="Z21" t="inlineStr"/>
       <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr">
+      <c r="AB21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr">
         <is>
           <t>insufficient sample size, poor methodology</t>
         </is>
       </c>
-      <c r="AC21" t="inlineStr"/>
       <c r="AD21" t="inlineStr"/>
       <c r="AE21" t="inlineStr"/>
       <c r="AF21" t="inlineStr"/>
       <c r="AG21" t="inlineStr"/>
-      <c r="AH21" t="inlineStr">
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr">
         <is>
           <t>poor methodology</t>
         </is>
       </c>
-      <c r="AI21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 12:43:52
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,11 +3822,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>coco</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 18:28:57
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3822,7 +3822,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:01:30
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3827,7 +3827,11 @@
           <t>cc</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr"/>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>dd</t>
+        </is>
+      </c>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:02:07
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,16 +3822,8 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>cc</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>dd</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:02:28
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,7 +3822,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>qw</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:03:08
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,11 +3822,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>qw</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:04:02
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,7 +3822,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>we</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 13:04:27
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3822,11 +3822,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>we</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 18:20:55
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3824,7 +3824,11 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>rejected</t>
+        </is>
+      </c>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update screening data - 2025-06-16 18:21:19
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -3824,11 +3824,7 @@
       </c>
       <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>rejected</t>
-        </is>
-      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
Update screening data - 2025-07-05 10:07:42
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3822,7 +3822,11 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr"/>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>

<commit_message>
Update screening data - 2025-07-05 04:42:17
</commit_message>
<xml_diff>
--- a/screening_criteria_dataset.xlsx
+++ b/screening_criteria_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3822,11 +3822,7 @@
           <t>Rejection reasons</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>test1</t>
-        </is>
-      </c>
+      <c r="C21" t="inlineStr"/>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr"/>
       <c r="F21" t="inlineStr"/>

</xml_diff>